<commit_message>
selenium loop per pages
</commit_message>
<xml_diff>
--- a/Taiwan Clients 2023.08.23.xlsx
+++ b/Taiwan Clients 2023.08.23.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ocean\OneDrive\桌面\work\dataCawlingLibrary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ocean\OneDrive\桌面\work\webDataCawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC0A5D1-987C-4311-BB21-C74E8C115487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0499A9AA-093C-4FE4-92F4-2F7A653581EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{EFE63C5A-48A8-4B1C-935F-E835E67EA390}"/>
+    <workbookView xWindow="437" yWindow="1346" windowWidth="23846" windowHeight="12000" xr2:uid="{EFE63C5A-48A8-4B1C-935F-E835E67EA390}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -552,7 +552,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.45" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Fin get at aspeedtech
</commit_message>
<xml_diff>
--- a/Taiwan Clients 2023.08.23.xlsx
+++ b/Taiwan Clients 2023.08.23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ocean\OneDrive\桌面\work\webDataCawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0499A9AA-093C-4FE4-92F4-2F7A653581EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15854AFD-29F9-42D6-B709-EB74C9CBE793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="437" yWindow="1346" windowWidth="23846" windowHeight="12000" xr2:uid="{EFE63C5A-48A8-4B1C-935F-E835E67EA390}"/>
   </bookViews>
@@ -552,7 +552,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.45" x14ac:dyDescent="0.4"/>

</xml_diff>